<commit_message>
Completed functional makefile template for modules.
</commit_message>
<xml_diff>
--- a/doc/Fortran Port Tasklist.xlsx
+++ b/doc/Fortran Port Tasklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Task #</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Create makefile and directory organization for smooth workflow</t>
   </si>
   <si>
-    <t>Creating directories and makefile modifications for Debug and Release modes.</t>
-  </si>
-  <si>
     <t>Read in data from text files</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Create a catalog of the C++ code's functionalities that need to be ported to Fortran</t>
   </si>
   <si>
-    <t>Includes reading array size metadata and geometry-specific text files.</t>
-  </si>
-  <si>
     <t>Create variables, structures, classes, etc.</t>
   </si>
   <si>
@@ -67,6 +61,15 @@
   </si>
   <si>
     <t>Potential room for performance and/or readability improvement.</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Functionally completed, with room for improvement down the line</t>
+  </si>
+  <si>
+    <t>Includes reading array size metadata and geometry-specific text files. Had to figure out modules and compilation first.</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,7 +437,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="108.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -442,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>44475</v>
+        <v>44490</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -456,7 +459,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
@@ -470,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5">
         <v>0.95</v>
@@ -484,16 +487,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="5">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -504,13 +507,13 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="5">
         <v>0.1</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -518,16 +521,16 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished code to read input files and updated documentation.
</commit_message>
<xml_diff>
--- a/doc/Fortran Port Tasklist.xlsx
+++ b/doc/Fortran Port Tasklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Task #</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Paused</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Create makefile and directory organization for smooth workflow</t>
   </si>
   <si>
@@ -69,7 +66,7 @@
     <t>Functionally completed, with room for improvement down the line</t>
   </si>
   <si>
-    <t>Includes reading array size metadata and geometry-specific text files. Had to figure out modules and compilation first.</t>
+    <t>Includes reading array size metadata and geometry-specific input files. Improvements could be made to pre-processing structure.</t>
   </si>
 </sst>
 </file>
@@ -428,7 +425,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +456,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
@@ -473,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="5">
         <v>0.95</v>
@@ -487,16 +484,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -504,16 +501,16 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -521,16 +518,16 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added variable definition file, updated documentation, begin work on config file
</commit_message>
<xml_diff>
--- a/doc/Fortran Port Tasklist.xlsx
+++ b/doc/Fortran Port Tasklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Task #</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Read in data from text files</t>
   </si>
   <si>
-    <t>Upcoming</t>
-  </si>
-  <si>
     <t>Create a catalog of the C++ code's functionalities that need to be ported to Fortran</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Completion</t>
   </si>
   <si>
-    <t>Potential room for performance and/or readability improvement.</t>
-  </si>
-  <si>
     <t>Completed</t>
   </si>
   <si>
@@ -67,6 +61,33 @@
   </si>
   <si>
     <t>Includes reading array size metadata and geometry-specific input files. Improvements could be made to pre-processing structure.</t>
+  </si>
+  <si>
+    <t>Most important variables created in simple arrays instead of complex structures. Variables will be defined as necessary.</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Create configuration file</t>
+  </si>
+  <si>
+    <t>Localize simulation configuration to one place, instead of having to check multiple places before running (like in the C++ code)</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>Allocate and initialize variables</t>
+  </si>
+  <si>
+    <t>Initialize simulation</t>
+  </si>
+  <si>
+    <t>Enforce boundary conditions on initial conditions</t>
+  </si>
+  <si>
+    <t>Calculate flow derivatives</t>
   </si>
 </sst>
 </file>
@@ -422,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>44490</v>
+        <v>44517</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -456,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
@@ -470,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="5">
         <v>0.95</v>
@@ -484,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -493,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -501,7 +522,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -510,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -518,16 +539,77 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>6.01</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>6.02</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>6.03</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C++ boundary conditions ported, with documentation
</commit_message>
<xml_diff>
--- a/doc/Fortran Port Tasklist.xlsx
+++ b/doc/Fortran Port Tasklist.xlsx
@@ -475,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>44538</v>
+        <v>44588</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -630,13 +630,13 @@
         <v>7.02</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,10 +644,13 @@
         <v>7.03</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>